<commit_message>
Toelichting gegeven van resultaten aan de onderkant van de sheet
</commit_message>
<xml_diff>
--- a/Eindopdracht/analyse.xlsx
+++ b/Eindopdracht/analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\School\HPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB659000-1ED8-47A8-94C3-9D638240A62B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC831BD-E66B-4EDE-8222-A3C7B0B3DDAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4215" windowWidth="28800" windowHeight="11385" xr2:uid="{2EFF1824-40F7-41DB-A122-ECAC5515EB16}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>List size</t>
   </si>
@@ -79,6 +79,21 @@
   </si>
   <si>
     <t>Tijd</t>
+  </si>
+  <si>
+    <t>Mijn sequentiele zeef gebruikt booleans, en is compleet anders geimplementeerd dan mijn MPI versie. Daarom vind ik dat ik</t>
+  </si>
+  <si>
+    <t>dat ik de twee versies niet echt kan vergelijken, omdat ze op een compleet andere manier het probleem aanpakken.</t>
+  </si>
+  <si>
+    <t>Mijn sequentiele versie is veel sneller dan mijn MP versie. De sequentiele versie doet er ruim 9 seconden over om 1 miljard waardes te checken.</t>
+  </si>
+  <si>
+    <t>De MP versie, doet er nog 20 seconden over om 1 miljoen te tellen.</t>
+  </si>
+  <si>
+    <t>ssssssssss</t>
   </si>
 </sst>
 </file>
@@ -2685,10 +2700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF7305B-2FD8-4BCA-849A-2D3E7775CF0A}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2983,6 +2998,31 @@
         <v>9.3964934349060005</v>
       </c>
     </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>